<commit_message>
Update: Final Project Plan
</commit_message>
<xml_diff>
--- a/Documents/Project_Plan/Caffeine_Project_Schedule.xlsx
+++ b/Documents/Project_Plan/Caffeine_Project_Schedule.xlsx
@@ -602,9 +602,8 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="3">
-        <f>IF(WEEKDAY(B4)=6,B4+ 3,B4+ 1)</f>
-        <v>45670</v>
+      <c r="B5" s="6">
+        <v>45672.0</v>
       </c>
       <c r="C5" s="7">
         <v>14.0</v>
@@ -640,7 +639,7 @@
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="6">
-        <v>45672.0</v>
+        <v>45674.0</v>
       </c>
       <c r="C6" s="7">
         <v>14.0</v>
@@ -676,7 +675,7 @@
     <row r="7" ht="13.5" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="6">
-        <v>45677.0</v>
+        <v>45679.0</v>
       </c>
       <c r="C7" s="7">
         <v>14.0</v>
@@ -712,7 +711,7 @@
     <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="6">
-        <v>45679.0</v>
+        <v>45681.0</v>
       </c>
       <c r="C8" s="7">
         <v>14.0</v>

</xml_diff>

<commit_message>
Update document: Project Plan
</commit_message>
<xml_diff>
--- a/Documents/Project_Plan/Caffeine_Project_Schedule.xlsx
+++ b/Documents/Project_Plan/Caffeine_Project_Schedule.xlsx
@@ -3,22 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Team 1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="V1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Team 1'!$B$2:$F$20</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'V1'!$B$2:$F$29</definedName>
   </definedNames>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="4EnAb3lItHzAqjxJRdRMGckEMPeDZaHNFNVV5KqR6VI="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="nzLkuwyocuj/mMwkMIsNSiORln7XVviuROUXagFnMh4="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -35,64 +35,112 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Member</t>
+  </si>
+  <si>
     <t>09:00-23:00</t>
   </si>
   <si>
-    <t>Mock Project - Day 1 - Kick off + Create requirement outline + Project Plan</t>
+    <t>Mock Project  - Kick off + Create requirement outline + Project Plan</t>
   </si>
   <si>
-    <t>Started</t>
+    <t>Done</t>
   </si>
   <si>
-    <t>Mock Project - Day 2 - Create SRS</t>
+    <t>All member</t>
   </si>
   <si>
-    <t>Mock Project - Day 3 - Review and update SRS</t>
+    <t>Mock Project  - Create SRS</t>
   </si>
   <si>
-    <t>Mock Project - Day 4 - Database Design + Review Database Design</t>
+    <t>Mock Project - Review and update SRS</t>
   </si>
   <si>
-    <t>Mock Project - Day 5 - Create Blackbox Testcase</t>
+    <t>Mock Project - Database Design + Review Database Design</t>
   </si>
   <si>
-    <t>Mock Project - Day 6 - Review and update Blackbox TC</t>
+    <t>Mock Project - Create Blackbox Testcase</t>
+  </si>
+  <si>
+    <t>Mock Project  - Review and update Blackbox TC</t>
   </si>
   <si>
     <t>off tet</t>
   </si>
   <si>
-    <t>Mock Project - Day 7 - Coding</t>
+    <t>Coding - Authenticate/Authorize</t>
   </si>
   <si>
-    <t>Mock Project - Day 8 - Coding</t>
+    <t>Khôi</t>
   </si>
   <si>
-    <t>Mock Project - Day 9 - Coding</t>
+    <t>CRUD beverage</t>
   </si>
   <si>
-    <t>Mock Project - Day 10 - Coding</t>
+    <t>Hải</t>
   </si>
   <si>
-    <t>Mock Project - Day 11 - Coding</t>
+    <t>CRUD staff</t>
   </si>
   <si>
-    <t>Mock Project - Day 12 - Review code + UT</t>
+    <t>Triều</t>
   </si>
   <si>
-    <t>Mock Project - Day 13 - UT</t>
+    <t>CRUD promotion</t>
   </si>
   <si>
-    <t>Mock Project - Day 14 - IT</t>
+    <t>Thi</t>
   </si>
   <si>
-    <t>Mock Project - Day 15 - IT + Create Test Report</t>
+    <t>CRUD inventory</t>
   </si>
   <si>
-    <t>Mock Project - Day 16 - Final Report</t>
+    <t>Huỳnh</t>
   </si>
   <si>
-    <t>Mock Project - Day 17 - Final Report (cont)</t>
+    <t>Set table - Update table</t>
+  </si>
+  <si>
+    <t>Update profile</t>
+  </si>
+  <si>
+    <t>Create bill</t>
+  </si>
+  <si>
+    <t>Export inventory data</t>
+  </si>
+  <si>
+    <t>View revenue</t>
+  </si>
+  <si>
+    <t>View salary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Request shift </t>
+  </si>
+  <si>
+    <t>Accept shift</t>
+  </si>
+  <si>
+    <t>Export revenue report</t>
+  </si>
+  <si>
+    <t>Mock Project  - Review code + UT</t>
+  </si>
+  <si>
+    <t>Mock Project  - UT</t>
+  </si>
+  <si>
+    <t>Mock Project  - IT</t>
+  </si>
+  <si>
+    <t>Mock Project  - IT + Create Test Report</t>
+  </si>
+  <si>
+    <t>Mock Project - Final Report</t>
+  </si>
+  <si>
+    <t>Mock Project - Final Report (cont)</t>
   </si>
   <si>
     <t>Tên đề tài:</t>
@@ -189,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -199,6 +247,9 @@
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -207,6 +258,9 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="16" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="center"/>
@@ -455,9 +509,10 @@
     <col customWidth="1" min="2" max="2" width="17.57"/>
     <col customWidth="1" min="3" max="3" width="19.57"/>
     <col customWidth="1" min="4" max="4" width="17.57"/>
-    <col customWidth="1" min="5" max="5" width="71.29"/>
+    <col customWidth="1" min="5" max="5" width="84.14"/>
     <col customWidth="1" min="6" max="6" width="16.71"/>
-    <col customWidth="1" min="7" max="26" width="9.0"/>
+    <col customWidth="1" min="7" max="7" width="19.86"/>
+    <col customWidth="1" min="8" max="26" width="9.0"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
@@ -505,7 +560,9 @@
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -528,22 +585,24 @@
     </row>
     <row r="3" ht="13.5" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>45666.0</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="5">
         <v>14.0</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="F3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -566,20 +625,24 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="6">
+      <c r="B4" s="8">
         <v>45667.0</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="9">
         <v>14.0</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>5</v>
+      <c r="D4" s="6" t="s">
+        <v>6</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="1"/>
+      <c r="G4" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -602,20 +665,24 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="6">
+      <c r="B5" s="8">
         <v>45672.0</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="9">
         <v>14.0</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>5</v>
+      <c r="D5" s="6" t="s">
+        <v>6</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -638,20 +705,22 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="6">
+      <c r="B6" s="8">
         <v>45674.0</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="9">
         <v>14.0</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>5</v>
+      <c r="D6" s="6" t="s">
+        <v>6</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>10</v>
+      <c r="E6" s="5" t="s">
+        <v>12</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="1"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -674,20 +743,22 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="6">
+      <c r="B7" s="8">
         <v>45679.0</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="9">
         <v>14.0</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>5</v>
+      <c r="D7" s="6" t="s">
+        <v>6</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>11</v>
+      <c r="E7" s="5" t="s">
+        <v>13</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="1"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -710,20 +781,22 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="6">
+      <c r="B8" s="8">
         <v>45681.0</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="9">
         <v>14.0</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>5</v>
+      <c r="D8" s="6" t="s">
+        <v>6</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>12</v>
+      <c r="E8" s="5" t="s">
+        <v>14</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="1"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -746,14 +819,14 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="8" t="s">
-        <v>13</v>
+      <c r="B9" s="10" t="s">
+        <v>15</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="1"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="7"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -776,20 +849,22 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="6">
-        <v>45693.0</v>
+      <c r="B10" s="8">
+        <v>45697.0</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="9">
         <v>14.0</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>5</v>
+      <c r="D10" s="6" t="s">
+        <v>6</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>14</v>
+      <c r="E10" s="5" t="s">
+        <v>16</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="1"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -812,20 +887,16 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="6">
-        <v>45700.0</v>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="5" t="s">
+        <v>18</v>
       </c>
-      <c r="C11" s="7">
-        <v>14.0</v>
+      <c r="F11" s="9"/>
+      <c r="G11" s="7" t="s">
+        <v>19</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -848,20 +919,16 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="6">
-        <v>45707.0</v>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="5" t="s">
+        <v>20</v>
       </c>
-      <c r="C12" s="7">
-        <v>14.0</v>
+      <c r="F12" s="9"/>
+      <c r="G12" s="7" t="s">
+        <v>21</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -884,20 +951,16 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="6">
-        <v>45714.0</v>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="5" t="s">
+        <v>22</v>
       </c>
-      <c r="C13" s="7">
-        <v>14.0</v>
+      <c r="F13" s="9"/>
+      <c r="G13" s="7" t="s">
+        <v>23</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -920,20 +983,16 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="6">
-        <v>45720.0</v>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="5" t="s">
+        <v>24</v>
       </c>
-      <c r="C14" s="7">
-        <v>14.0</v>
+      <c r="F14" s="9"/>
+      <c r="G14" s="7" t="s">
+        <v>25</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -956,20 +1015,22 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="6">
-        <v>45727.0</v>
+      <c r="B15" s="8">
+        <v>45707.0</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="9">
         <v>14.0</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>5</v>
+      <c r="D15" s="6" t="s">
+        <v>6</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>19</v>
+      <c r="E15" s="5" t="s">
+        <v>26</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="1"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -992,20 +1053,16 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="6">
-        <v>45732.0</v>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="5" t="s">
+        <v>27</v>
       </c>
-      <c r="C16" s="7">
-        <v>14.0</v>
+      <c r="F16" s="9"/>
+      <c r="G16" s="7" t="s">
+        <v>19</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1028,20 +1085,16 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="6">
-        <v>45737.0</v>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="5" t="s">
+        <v>28</v>
       </c>
-      <c r="C17" s="7">
-        <v>14.0</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="7" t="s">
+      <c r="F17" s="9"/>
+      <c r="G17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1064,20 +1117,16 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="6">
-        <v>45740.0</v>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="5" t="s">
+        <v>29</v>
       </c>
-      <c r="C18" s="7">
-        <v>14.0</v>
+      <c r="F18" s="9"/>
+      <c r="G18" s="7" t="s">
+        <v>25</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1100,20 +1149,16 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="6">
-        <v>45745.0</v>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="5" t="s">
+        <v>30</v>
       </c>
-      <c r="C19" s="7">
-        <v>14.0</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="7" t="s">
+      <c r="F19" s="9"/>
+      <c r="G19" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1136,21 +1181,22 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="3">
-        <f>IF(WEEKDAY(B19)=6,B19+ 3,B19+ 1)</f>
-        <v>45746</v>
+      <c r="B20" s="8">
+        <v>45720.0</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="9">
         <v>14.0</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>5</v>
+      <c r="D20" s="6" t="s">
+        <v>6</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>24</v>
+      <c r="E20" s="5" t="s">
+        <v>31</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="1"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1173,12 +1219,16 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -1201,12 +1251,16 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1229,16 +1283,16 @@
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="11" t="s">
-        <v>25</v>
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="5" t="s">
+        <v>34</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>26</v>
+      <c r="F23" s="9"/>
+      <c r="G23" s="7" t="s">
+        <v>9</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1261,12 +1315,22 @@
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="B24" s="8">
+        <v>45727.0</v>
+      </c>
+      <c r="C24" s="9">
+        <v>14.0</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1289,12 +1353,22 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="B25" s="8">
+        <v>45732.0</v>
+      </c>
+      <c r="C25" s="9">
+        <v>14.0</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="9"/>
+      <c r="G25" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1317,11 +1391,22 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="B26" s="8">
+        <v>45737.0</v>
+      </c>
+      <c r="C26" s="9">
+        <v>14.0</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1344,11 +1429,22 @@
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="B27" s="8">
+        <v>45740.0</v>
+      </c>
+      <c r="C27" s="9">
+        <v>14.0</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1371,11 +1467,19 @@
     </row>
     <row r="28" ht="13.5" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="B28" s="8">
+        <v>45745.0</v>
+      </c>
+      <c r="C28" s="9">
+        <v>14.0</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="9"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -1399,10 +1503,20 @@
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="B29" s="4">
+        <f>IF(WEEKDAY(B28)=6,B28+ 3,B28+ 1)</f>
+        <v>45746</v>
+      </c>
+      <c r="C29" s="9">
+        <v>14.0</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="9"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -1482,8 +1596,12 @@
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+      <c r="B32" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>42</v>
+      </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1566,8 +1684,7 @@
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+      <c r="C35" s="15"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -1594,8 +1711,7 @@
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="C36" s="15"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -1622,8 +1738,8 @@
     </row>
     <row r="37" ht="13.5" customHeight="1">
       <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="15"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -1650,8 +1766,7 @@
     </row>
     <row r="38" ht="13.5" customHeight="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
+      <c r="C38" s="15"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -28640,10 +28755,265 @@
       <c r="Y1001" s="1"/>
       <c r="Z1001" s="1"/>
     </row>
+    <row r="1002" ht="13.5" customHeight="1">
+      <c r="A1002" s="1"/>
+      <c r="B1002" s="1"/>
+      <c r="C1002" s="1"/>
+      <c r="D1002" s="1"/>
+      <c r="E1002" s="1"/>
+      <c r="F1002" s="1"/>
+      <c r="G1002" s="1"/>
+      <c r="H1002" s="1"/>
+      <c r="I1002" s="1"/>
+      <c r="J1002" s="1"/>
+      <c r="K1002" s="1"/>
+      <c r="L1002" s="1"/>
+      <c r="M1002" s="1"/>
+      <c r="N1002" s="1"/>
+      <c r="O1002" s="1"/>
+      <c r="P1002" s="1"/>
+      <c r="Q1002" s="1"/>
+      <c r="R1002" s="1"/>
+      <c r="S1002" s="1"/>
+      <c r="T1002" s="1"/>
+      <c r="U1002" s="1"/>
+      <c r="V1002" s="1"/>
+      <c r="W1002" s="1"/>
+      <c r="X1002" s="1"/>
+      <c r="Y1002" s="1"/>
+      <c r="Z1002" s="1"/>
+    </row>
+    <row r="1003" ht="13.5" customHeight="1">
+      <c r="A1003" s="1"/>
+      <c r="B1003" s="1"/>
+      <c r="C1003" s="1"/>
+      <c r="D1003" s="1"/>
+      <c r="E1003" s="1"/>
+      <c r="F1003" s="1"/>
+      <c r="G1003" s="1"/>
+      <c r="H1003" s="1"/>
+      <c r="I1003" s="1"/>
+      <c r="J1003" s="1"/>
+      <c r="K1003" s="1"/>
+      <c r="L1003" s="1"/>
+      <c r="M1003" s="1"/>
+      <c r="N1003" s="1"/>
+      <c r="O1003" s="1"/>
+      <c r="P1003" s="1"/>
+      <c r="Q1003" s="1"/>
+      <c r="R1003" s="1"/>
+      <c r="S1003" s="1"/>
+      <c r="T1003" s="1"/>
+      <c r="U1003" s="1"/>
+      <c r="V1003" s="1"/>
+      <c r="W1003" s="1"/>
+      <c r="X1003" s="1"/>
+      <c r="Y1003" s="1"/>
+      <c r="Z1003" s="1"/>
+    </row>
+    <row r="1004" ht="13.5" customHeight="1">
+      <c r="A1004" s="1"/>
+      <c r="B1004" s="1"/>
+      <c r="C1004" s="1"/>
+      <c r="D1004" s="1"/>
+      <c r="E1004" s="1"/>
+      <c r="F1004" s="1"/>
+      <c r="G1004" s="1"/>
+      <c r="H1004" s="1"/>
+      <c r="I1004" s="1"/>
+      <c r="J1004" s="1"/>
+      <c r="K1004" s="1"/>
+      <c r="L1004" s="1"/>
+      <c r="M1004" s="1"/>
+      <c r="N1004" s="1"/>
+      <c r="O1004" s="1"/>
+      <c r="P1004" s="1"/>
+      <c r="Q1004" s="1"/>
+      <c r="R1004" s="1"/>
+      <c r="S1004" s="1"/>
+      <c r="T1004" s="1"/>
+      <c r="U1004" s="1"/>
+      <c r="V1004" s="1"/>
+      <c r="W1004" s="1"/>
+      <c r="X1004" s="1"/>
+      <c r="Y1004" s="1"/>
+      <c r="Z1004" s="1"/>
+    </row>
+    <row r="1005" ht="13.5" customHeight="1">
+      <c r="A1005" s="1"/>
+      <c r="B1005" s="1"/>
+      <c r="C1005" s="1"/>
+      <c r="D1005" s="1"/>
+      <c r="E1005" s="1"/>
+      <c r="F1005" s="1"/>
+      <c r="G1005" s="1"/>
+      <c r="H1005" s="1"/>
+      <c r="I1005" s="1"/>
+      <c r="J1005" s="1"/>
+      <c r="K1005" s="1"/>
+      <c r="L1005" s="1"/>
+      <c r="M1005" s="1"/>
+      <c r="N1005" s="1"/>
+      <c r="O1005" s="1"/>
+      <c r="P1005" s="1"/>
+      <c r="Q1005" s="1"/>
+      <c r="R1005" s="1"/>
+      <c r="S1005" s="1"/>
+      <c r="T1005" s="1"/>
+      <c r="U1005" s="1"/>
+      <c r="V1005" s="1"/>
+      <c r="W1005" s="1"/>
+      <c r="X1005" s="1"/>
+      <c r="Y1005" s="1"/>
+      <c r="Z1005" s="1"/>
+    </row>
+    <row r="1006" ht="13.5" customHeight="1">
+      <c r="A1006" s="1"/>
+      <c r="B1006" s="1"/>
+      <c r="C1006" s="1"/>
+      <c r="D1006" s="1"/>
+      <c r="E1006" s="1"/>
+      <c r="F1006" s="1"/>
+      <c r="G1006" s="1"/>
+      <c r="H1006" s="1"/>
+      <c r="I1006" s="1"/>
+      <c r="J1006" s="1"/>
+      <c r="K1006" s="1"/>
+      <c r="L1006" s="1"/>
+      <c r="M1006" s="1"/>
+      <c r="N1006" s="1"/>
+      <c r="O1006" s="1"/>
+      <c r="P1006" s="1"/>
+      <c r="Q1006" s="1"/>
+      <c r="R1006" s="1"/>
+      <c r="S1006" s="1"/>
+      <c r="T1006" s="1"/>
+      <c r="U1006" s="1"/>
+      <c r="V1006" s="1"/>
+      <c r="W1006" s="1"/>
+      <c r="X1006" s="1"/>
+      <c r="Y1006" s="1"/>
+      <c r="Z1006" s="1"/>
+    </row>
+    <row r="1007" ht="13.5" customHeight="1">
+      <c r="A1007" s="1"/>
+      <c r="B1007" s="1"/>
+      <c r="C1007" s="1"/>
+      <c r="D1007" s="1"/>
+      <c r="E1007" s="1"/>
+      <c r="F1007" s="1"/>
+      <c r="G1007" s="1"/>
+      <c r="H1007" s="1"/>
+      <c r="I1007" s="1"/>
+      <c r="J1007" s="1"/>
+      <c r="K1007" s="1"/>
+      <c r="L1007" s="1"/>
+      <c r="M1007" s="1"/>
+      <c r="N1007" s="1"/>
+      <c r="O1007" s="1"/>
+      <c r="P1007" s="1"/>
+      <c r="Q1007" s="1"/>
+      <c r="R1007" s="1"/>
+      <c r="S1007" s="1"/>
+      <c r="T1007" s="1"/>
+      <c r="U1007" s="1"/>
+      <c r="V1007" s="1"/>
+      <c r="W1007" s="1"/>
+      <c r="X1007" s="1"/>
+      <c r="Y1007" s="1"/>
+      <c r="Z1007" s="1"/>
+    </row>
+    <row r="1008" ht="13.5" customHeight="1">
+      <c r="A1008" s="1"/>
+      <c r="B1008" s="1"/>
+      <c r="C1008" s="1"/>
+      <c r="D1008" s="1"/>
+      <c r="E1008" s="1"/>
+      <c r="F1008" s="1"/>
+      <c r="G1008" s="1"/>
+      <c r="H1008" s="1"/>
+      <c r="I1008" s="1"/>
+      <c r="J1008" s="1"/>
+      <c r="K1008" s="1"/>
+      <c r="L1008" s="1"/>
+      <c r="M1008" s="1"/>
+      <c r="N1008" s="1"/>
+      <c r="O1008" s="1"/>
+      <c r="P1008" s="1"/>
+      <c r="Q1008" s="1"/>
+      <c r="R1008" s="1"/>
+      <c r="S1008" s="1"/>
+      <c r="T1008" s="1"/>
+      <c r="U1008" s="1"/>
+      <c r="V1008" s="1"/>
+      <c r="W1008" s="1"/>
+      <c r="X1008" s="1"/>
+      <c r="Y1008" s="1"/>
+      <c r="Z1008" s="1"/>
+    </row>
+    <row r="1009" ht="13.5" customHeight="1">
+      <c r="A1009" s="1"/>
+      <c r="B1009" s="1"/>
+      <c r="C1009" s="1"/>
+      <c r="D1009" s="1"/>
+      <c r="E1009" s="1"/>
+      <c r="F1009" s="1"/>
+      <c r="G1009" s="1"/>
+      <c r="H1009" s="1"/>
+      <c r="I1009" s="1"/>
+      <c r="J1009" s="1"/>
+      <c r="K1009" s="1"/>
+      <c r="L1009" s="1"/>
+      <c r="M1009" s="1"/>
+      <c r="N1009" s="1"/>
+      <c r="O1009" s="1"/>
+      <c r="P1009" s="1"/>
+      <c r="Q1009" s="1"/>
+      <c r="R1009" s="1"/>
+      <c r="S1009" s="1"/>
+      <c r="T1009" s="1"/>
+      <c r="U1009" s="1"/>
+      <c r="V1009" s="1"/>
+      <c r="W1009" s="1"/>
+      <c r="X1009" s="1"/>
+      <c r="Y1009" s="1"/>
+      <c r="Z1009" s="1"/>
+    </row>
+    <row r="1010" ht="13.5" customHeight="1">
+      <c r="A1010" s="1"/>
+      <c r="B1010" s="1"/>
+      <c r="C1010" s="1"/>
+      <c r="D1010" s="1"/>
+      <c r="E1010" s="1"/>
+      <c r="F1010" s="1"/>
+      <c r="G1010" s="1"/>
+      <c r="H1010" s="1"/>
+      <c r="I1010" s="1"/>
+      <c r="J1010" s="1"/>
+      <c r="K1010" s="1"/>
+      <c r="L1010" s="1"/>
+      <c r="M1010" s="1"/>
+      <c r="N1010" s="1"/>
+      <c r="O1010" s="1"/>
+      <c r="P1010" s="1"/>
+      <c r="Q1010" s="1"/>
+      <c r="R1010" s="1"/>
+      <c r="S1010" s="1"/>
+      <c r="T1010" s="1"/>
+      <c r="U1010" s="1"/>
+      <c r="V1010" s="1"/>
+      <c r="W1010" s="1"/>
+      <c r="X1010" s="1"/>
+      <c r="Y1010" s="1"/>
+      <c r="Z1010" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$B$2:$F$20"/>
+  <autoFilter ref="$B$2:$F$29"/>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F3:F20">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G3:G8 G10:G27">
+      <formula1>"Khôi,Thi,Triều,Hải,Huỳnh,All member"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F3:F29">
       <formula1>"Started,Pending,Done,Cancel"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>